<commit_message>
complete 列名のみかたfor aggregate files
</commit_message>
<xml_diff>
--- a/Suzuki_and_Nakata_mini/列名のみかた.xlsx
+++ b/Suzuki_and_Nakata_mini/列名のみかた.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Documents\codes\private_tasks\鈴木・中田さんのデータ整形\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\L-YN1409-u\Documents\share\Suzuki_and_Nakata_mini\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CB8029B1-B653-4083-BEAA-E443B2E0C694}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="2730" windowWidth="20865" windowHeight="11835" activeTab="1" xr2:uid="{D95DA89F-BACB-4906-A86F-4036AFC0603F}"/>
+    <workbookView xWindow="4650" yWindow="2730" windowWidth="20865" windowHeight="11835" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="S" sheetId="1" r:id="rId1"/>
-    <sheet name="N" sheetId="2" r:id="rId2"/>
+    <sheet name="鈴木" sheetId="1" r:id="rId1"/>
+    <sheet name="中田" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="123">
   <si>
     <t>id</t>
   </si>
@@ -253,19 +252,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>直前にLOSEだったときの，ハイリスク選択率</t>
-    <rPh sb="0" eb="2">
-      <t>チョクゼン</t>
-    </rPh>
-    <rPh sb="19" eb="21">
-      <t>センタク</t>
-    </rPh>
-    <rPh sb="21" eb="22">
-      <t>リツ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>直前がLOSEだった試行回数</t>
     <rPh sb="0" eb="2">
       <t>チョクゼン</t>
@@ -279,19 +265,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>直前にGAINだったときの，ハイリスク選択率</t>
-    <rPh sb="0" eb="2">
-      <t>チョクゼン</t>
-    </rPh>
-    <rPh sb="19" eb="21">
-      <t>センタク</t>
-    </rPh>
-    <rPh sb="21" eb="22">
-      <t>リツ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>直前がGAINだった試行回数</t>
     <rPh sb="0" eb="2">
       <t>チョクゼン</t>
@@ -305,19 +278,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>直前にL10だったときの，ハイリスク選択率</t>
-    <rPh sb="0" eb="2">
-      <t>チョクゼン</t>
-    </rPh>
-    <rPh sb="18" eb="20">
-      <t>センタク</t>
-    </rPh>
-    <rPh sb="20" eb="21">
-      <t>リツ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>直前がL10だった試行回数</t>
     <rPh sb="0" eb="2">
       <t>チョクゼン</t>
@@ -331,19 +291,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>直前にG10だったときの，ハイリスク選択率</t>
-    <rPh sb="0" eb="2">
-      <t>チョクゼン</t>
-    </rPh>
-    <rPh sb="18" eb="20">
-      <t>センタク</t>
-    </rPh>
-    <rPh sb="20" eb="21">
-      <t>リツ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>直前がG10だった試行回数</t>
     <rPh sb="0" eb="2">
       <t>チョクゼン</t>
@@ -357,19 +304,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>直前にL50だったときの，ハイリスク選択率</t>
-    <rPh sb="0" eb="2">
-      <t>チョクゼン</t>
-    </rPh>
-    <rPh sb="18" eb="20">
-      <t>センタク</t>
-    </rPh>
-    <rPh sb="20" eb="21">
-      <t>リツ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>直前がL50だった試行回数</t>
     <rPh sb="0" eb="2">
       <t>チョクゼン</t>
@@ -383,19 +317,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>直前にG50だったときの，ハイリスク選択率</t>
-    <rPh sb="0" eb="2">
-      <t>チョクゼン</t>
-    </rPh>
-    <rPh sb="18" eb="20">
-      <t>センタク</t>
-    </rPh>
-    <rPh sb="20" eb="21">
-      <t>リツ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>直前がG50だった試行回数</t>
     <rPh sb="0" eb="2">
       <t>チョクゼン</t>
@@ -491,13 +412,215 @@
   </si>
   <si>
     <t>1: control, 2: soft, 3: hard</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>直前がLOSEだったときの，ハイリスク選択率</t>
+    <rPh sb="19" eb="21">
+      <t>センタク</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>リツ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>直前がGAINだったときの，ハイリスク選択率</t>
+    <rPh sb="19" eb="21">
+      <t>センタク</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>リツ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>直前がL10だったときの，ハイリスク選択率</t>
+    <rPh sb="18" eb="20">
+      <t>センタク</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>リツ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>直前がG10だったときの，ハイリスク選択率</t>
+    <rPh sb="18" eb="20">
+      <t>センタク</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>リツ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>直前がL50だったときの，ハイリスク選択率</t>
+    <rPh sb="18" eb="20">
+      <t>センタク</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>リツ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>直前がG50だったときの，ハイリスク選択率</t>
+    <rPh sb="18" eb="20">
+      <t>センタク</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>リツ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>１０点が外れたとき，どのように感じましたか？</t>
+  </si>
+  <si>
+    <t>１０点が当たったとき，どのように感じましたか？</t>
+  </si>
+  <si>
+    <t>５０点が外れたとき，どのように感じましたか？</t>
+  </si>
+  <si>
+    <t>５０点が当たったとき，どのように感じましたか？</t>
+  </si>
+  <si>
+    <t>敵意</t>
+    <rPh sb="0" eb="2">
+      <t>テキイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>抑うつ</t>
+    <rPh sb="0" eb="1">
+      <t>ヨク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>倦怠</t>
+    <rPh sb="0" eb="2">
+      <t>ケンタイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>活動的快</t>
+    <rPh sb="0" eb="3">
+      <t>カツドウテキ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>カイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>非活動的快</t>
+    <rPh sb="0" eb="1">
+      <t>ヒ</t>
+    </rPh>
+    <rPh sb="1" eb="4">
+      <t>カツドウテキ</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>カイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>親和</t>
+    <rPh sb="0" eb="2">
+      <t>シンワ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>集中</t>
+    <rPh sb="0" eb="2">
+      <t>シュウチュウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>驚愕</t>
+    <rPh sb="0" eb="2">
+      <t>キョウガク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>条件</t>
+    <rPh sb="0" eb="2">
+      <t>ジョウケン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>課題の前</t>
+    <rPh sb="0" eb="2">
+      <t>カダイ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>マエ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>前傾姿勢</t>
+    <rPh sb="0" eb="2">
+      <t>ゼンケイ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>シセイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>リクライニング姿勢</t>
+    <rPh sb="7" eb="9">
+      <t>シセイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>列名</t>
+    <rPh sb="0" eb="1">
+      <t>レツ</t>
+    </rPh>
+    <rPh sb="1" eb="2">
+      <t>メイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>中身</t>
+    <rPh sb="0" eb="2">
+      <t>ナカミ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>参加者ID</t>
+    <rPh sb="0" eb="3">
+      <t>サンカシャ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>共通</t>
+    <rPh sb="0" eb="2">
+      <t>キョウツウ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -852,11 +975,715 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5000790-F93C-49A3-B44A-177B2403FF44}">
-  <dimension ref="A1:B61"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1048576"/>
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.21875" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="35.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>116</v>
+      </c>
+      <c r="C8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>116</v>
+      </c>
+      <c r="C9" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>116</v>
+      </c>
+      <c r="C10" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" t="s">
+        <v>117</v>
+      </c>
+      <c r="C11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>117</v>
+      </c>
+      <c r="C13" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" t="s">
+        <v>117</v>
+      </c>
+      <c r="C14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" t="s">
+        <v>117</v>
+      </c>
+      <c r="C15" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
+        <v>117</v>
+      </c>
+      <c r="C16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" t="s">
+        <v>117</v>
+      </c>
+      <c r="C17" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" t="s">
+        <v>117</v>
+      </c>
+      <c r="C18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" t="s">
+        <v>117</v>
+      </c>
+      <c r="C19" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" t="s">
+        <v>117</v>
+      </c>
+      <c r="C20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" t="s">
+        <v>117</v>
+      </c>
+      <c r="C21" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" t="s">
+        <v>117</v>
+      </c>
+      <c r="C22" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" t="s">
+        <v>117</v>
+      </c>
+      <c r="C23" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" t="s">
+        <v>117</v>
+      </c>
+      <c r="C24" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" t="s">
+        <v>117</v>
+      </c>
+      <c r="C25" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" t="s">
+        <v>117</v>
+      </c>
+      <c r="C26" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" t="s">
+        <v>117</v>
+      </c>
+      <c r="C27" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" t="s">
+        <v>117</v>
+      </c>
+      <c r="C28" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29" t="s">
+        <v>117</v>
+      </c>
+      <c r="C29" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30" t="s">
+        <v>117</v>
+      </c>
+      <c r="C30" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>25</v>
+      </c>
+      <c r="B31" t="s">
+        <v>117</v>
+      </c>
+      <c r="C31" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" t="s">
+        <v>117</v>
+      </c>
+      <c r="C32" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>27</v>
+      </c>
+      <c r="B33" t="s">
+        <v>117</v>
+      </c>
+      <c r="C33" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>28</v>
+      </c>
+      <c r="B34" t="s">
+        <v>117</v>
+      </c>
+      <c r="C34" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>29</v>
+      </c>
+      <c r="B35" t="s">
+        <v>117</v>
+      </c>
+      <c r="C35" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>30</v>
+      </c>
+      <c r="B36" t="s">
+        <v>117</v>
+      </c>
+      <c r="C36" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>31</v>
+      </c>
+      <c r="B37" t="s">
+        <v>118</v>
+      </c>
+      <c r="C37" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38" t="s">
+        <v>118</v>
+      </c>
+      <c r="C38" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B39" t="s">
+        <v>118</v>
+      </c>
+      <c r="C39" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>34</v>
+      </c>
+      <c r="B40" t="s">
+        <v>118</v>
+      </c>
+      <c r="C40" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>35</v>
+      </c>
+      <c r="B41" t="s">
+        <v>118</v>
+      </c>
+      <c r="C41" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>36</v>
+      </c>
+      <c r="B42" t="s">
+        <v>118</v>
+      </c>
+      <c r="C42" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>37</v>
+      </c>
+      <c r="B43" t="s">
+        <v>118</v>
+      </c>
+      <c r="C43" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>38</v>
+      </c>
+      <c r="B44" t="s">
+        <v>118</v>
+      </c>
+      <c r="C44" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>39</v>
+      </c>
+      <c r="B45" t="s">
+        <v>118</v>
+      </c>
+      <c r="C45" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>40</v>
+      </c>
+      <c r="B46" t="s">
+        <v>118</v>
+      </c>
+      <c r="C46" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>41</v>
+      </c>
+      <c r="B47" t="s">
+        <v>118</v>
+      </c>
+      <c r="C47" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>42</v>
+      </c>
+      <c r="B48" t="s">
+        <v>118</v>
+      </c>
+      <c r="C48" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>43</v>
+      </c>
+      <c r="B49" t="s">
+        <v>118</v>
+      </c>
+      <c r="C49" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>44</v>
+      </c>
+      <c r="B50" t="s">
+        <v>118</v>
+      </c>
+      <c r="C50" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>45</v>
+      </c>
+      <c r="B51" t="s">
+        <v>118</v>
+      </c>
+      <c r="C51" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>46</v>
+      </c>
+      <c r="B52" t="s">
+        <v>118</v>
+      </c>
+      <c r="C52" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>47</v>
+      </c>
+      <c r="B53" t="s">
+        <v>118</v>
+      </c>
+      <c r="C53" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>48</v>
+      </c>
+      <c r="B54" t="s">
+        <v>118</v>
+      </c>
+      <c r="C54" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>49</v>
+      </c>
+      <c r="B55" t="s">
+        <v>118</v>
+      </c>
+      <c r="C55" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>50</v>
+      </c>
+      <c r="B56" t="s">
+        <v>118</v>
+      </c>
+      <c r="C56" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>51</v>
+      </c>
+      <c r="B57" t="s">
+        <v>118</v>
+      </c>
+      <c r="C57" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>52</v>
+      </c>
+      <c r="B58" t="s">
+        <v>118</v>
+      </c>
+      <c r="C58" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>53</v>
+      </c>
+      <c r="B59" t="s">
+        <v>118</v>
+      </c>
+      <c r="C59" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>54</v>
+      </c>
+      <c r="B60" t="s">
+        <v>118</v>
+      </c>
+      <c r="C60" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>55</v>
+      </c>
+      <c r="B61" t="s">
+        <v>118</v>
+      </c>
+      <c r="C61" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>56</v>
+      </c>
+      <c r="B62" t="s">
+        <v>118</v>
+      </c>
+      <c r="C62" t="s">
+        <v>114</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -867,108 +1694,135 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>119</v>
+      </c>
+      <c r="B1" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>69</v>
+      </c>
+      <c r="B3" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>70</v>
+      </c>
+      <c r="B4" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>71</v>
+      </c>
+      <c r="B5" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>72</v>
+      </c>
+      <c r="B6" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>73</v>
+      </c>
+      <c r="B7" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>74</v>
+      </c>
+      <c r="B8" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>75</v>
+      </c>
+      <c r="B9" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="B10" t="s">
-        <v>61</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="B11" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>78</v>
       </c>
       <c r="B12" t="s">
-        <v>63</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="B13" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
       <c r="B14" t="s">
-        <v>65</v>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>81</v>
       </c>
       <c r="B15" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>82</v>
       </c>
       <c r="B16" t="s">
-        <v>67</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="B17" t="s">
         <v>68</v>
@@ -976,446 +1830,98 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>84</v>
       </c>
       <c r="B18" t="s">
-        <v>69</v>
+        <v>103</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>85</v>
       </c>
       <c r="B19" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>86</v>
       </c>
       <c r="B20" t="s">
-        <v>71</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>87</v>
       </c>
       <c r="B21" t="s">
-        <v>72</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>88</v>
       </c>
       <c r="B22" t="s">
-        <v>73</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>18</v>
+        <v>89</v>
       </c>
       <c r="B23" t="s">
-        <v>74</v>
+        <v>107</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>19</v>
+        <v>90</v>
+      </c>
+      <c r="B24" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>20</v>
+        <v>91</v>
+      </c>
+      <c r="B25" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>21</v>
+        <v>92</v>
+      </c>
+      <c r="B26" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>22</v>
+        <v>93</v>
+      </c>
+      <c r="B27" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>23</v>
+        <v>94</v>
+      </c>
+      <c r="B28" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>56</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04A1D386-0F45-4903-A1F8-FADAFF441636}">
-  <dimension ref="A1:B28"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="28.21875" customWidth="1"/>
-    <col min="2" max="2" width="35.77734375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>80</v>
-      </c>
-      <c r="B7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>81</v>
-      </c>
-      <c r="B8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>82</v>
-      </c>
-      <c r="B9" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>83</v>
-      </c>
-      <c r="B10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>84</v>
-      </c>
-      <c r="B11" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>85</v>
-      </c>
-      <c r="B12" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>86</v>
-      </c>
-      <c r="B13" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>87</v>
-      </c>
-      <c r="B14" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>88</v>
-      </c>
-      <c r="B15" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>89</v>
-      </c>
-      <c r="B16" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>101</v>
+      <c r="B29" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>